<commit_message>
Modifiche riguardanti il cambio delle 4 variabili categoriche in fattori (Year non è una variabile numerica, ho eliminato Flag in quanto non è rilevante ai fini dell'indagine statistica, ho messo la library all'inizio, ho realizzato altri 4 barplot, basati su quelli precedenti per anni 2015, 2021, 2022 e un nuovo Barplot per fare un confronto
</commit_message>
<xml_diff>
--- a/Infant_Mortality.xlsx
+++ b/Infant_Mortality.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Documents\Università\Magistrale\SAD\Progetto_SAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17733716-F3F7-4C29-86B5-ADE9C8BD2E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847F417-30DD-419C-9CB8-FBDF63BFB5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:F2747"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>